<commit_message>
swati addded new classes
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ListManager_CreateList" sheetId="1" r:id="rId1"/>
@@ -146,9 +146,6 @@
     <t>BlackList_Email</t>
   </si>
   <si>
-    <t>swati@gmail.com</t>
-  </si>
-  <si>
     <t>BlackList_View_Email</t>
   </si>
   <si>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>294</t>
+  </si>
+  <si>
+    <t>swati45@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -552,7 +552,7 @@
         <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
         <v>21</v>
@@ -573,12 +573,12 @@
         <v>26</v>
       </c>
       <c r="K1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -587,10 +587,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
@@ -620,7 +620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -644,7 +644,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
         <v>27</v>
@@ -694,7 +694,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -706,7 +706,7 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -715,7 +715,7 @@
         <v>9</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K2" t="s">
         <v>10</v>
@@ -740,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +756,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
         <v>39</v>
@@ -765,13 +765,13 @@
         <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
         <v>42</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -782,7 +782,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -796,7 +796,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" display="swati@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>